<commit_message>
feat(ui): implement Material Design 3 theme with dark mode support
</commit_message>
<xml_diff>
--- a/homework_data.xlsx
+++ b/homework_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G172"/>
+  <dimension ref="A1:G176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3050,7 +3050,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>73523</t>
+          <t>73522</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -3073,7 +3073,7 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Grammar WB p.23</t>
+          <t>Notebook</t>
         </is>
       </c>
       <c r="G85" t="inlineStr"/>
@@ -3081,7 +3081,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>73522</t>
+          <t>記事6611</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -3104,7 +3104,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Notebook</t>
+          <t>Pre Vocab Quiz</t>
         </is>
       </c>
       <c r="G86" t="inlineStr"/>
@@ -3112,7 +3112,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>記事6611</t>
+          <t>73523</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -3135,7 +3135,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Pre Vocab Quiz</t>
+          <t>Grammar WB p.23</t>
         </is>
       </c>
       <c r="G87" t="inlineStr"/>
@@ -3205,12 +3205,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>記事6599</t>
+          <t>73609</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="C90" s="2" t="n">
@@ -3223,12 +3223,12 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>英文 -- ENG</t>
+          <t>數學 -- MATH</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Vocab Quiz</t>
+          <t>CW21</t>
         </is>
       </c>
       <c r="G90" t="inlineStr"/>
@@ -3236,12 +3236,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>73446</t>
+          <t>73610</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="C91" s="2" t="n">
@@ -3254,12 +3254,12 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>公經社 -- CES</t>
+          <t>英文 -- ENG</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>做書p.65</t>
+          <t>Grammar WB p.24-25</t>
         </is>
       </c>
       <c r="G91" t="inlineStr"/>
@@ -3267,12 +3267,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>記事6634</t>
+          <t>記事6599</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="C92" s="2" t="n">
@@ -3290,7 +3290,7 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Bring a glue</t>
+          <t>Vocab Quiz</t>
         </is>
       </c>
       <c r="G92" t="inlineStr"/>
@@ -3298,12 +3298,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>73610</t>
+          <t>73446</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-10</t>
         </is>
       </c>
       <c r="C93" s="2" t="n">
@@ -3316,12 +3316,12 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>英文 -- ENG</t>
+          <t>公經社 -- CES</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Grammar WB p.24-25</t>
+          <t>做書p.65</t>
         </is>
       </c>
       <c r="G93" t="inlineStr"/>
@@ -3329,7 +3329,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>73609</t>
+          <t>記事6634</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -3347,12 +3347,12 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>數學 -- MATH</t>
+          <t>英文 -- ENG</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>CW21</t>
+          <t>Bring a glue</t>
         </is>
       </c>
       <c r="G94" t="inlineStr"/>
@@ -3391,12 +3391,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>73709</t>
+          <t>73678</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="C96" s="2" t="n">
@@ -3409,12 +3409,12 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>數學 -- MATH</t>
+          <t>公經社 -- CES</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>CW22</t>
+          <t>WS連File</t>
         </is>
       </c>
       <c r="G96" t="inlineStr"/>
@@ -3453,12 +3453,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>73678</t>
+          <t>73709</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="C98" s="2" t="n">
@@ -3471,12 +3471,12 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>公經社 -- CES</t>
+          <t>數學 -- MATH</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>WS連File</t>
+          <t>CW22</t>
         </is>
       </c>
       <c r="G98" t="inlineStr"/>
@@ -3577,12 +3577,12 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>73673</t>
+          <t>73756</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="C102" s="2" t="n">
@@ -3595,12 +3595,12 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>科學 -- SCI</t>
+          <t>地理 -- GEOG</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>WB p.13 17 19</t>
+          <t>作業</t>
         </is>
       </c>
       <c r="G102" t="inlineStr"/>
@@ -3608,12 +3608,12 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>73757</t>
+          <t>73673</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="C103" s="2" t="n">
@@ -3626,12 +3626,12 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>數學 -- MATH</t>
+          <t>科學 -- SCI</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>HW 2C</t>
+          <t>WB p.13 17 19</t>
         </is>
       </c>
       <c r="G103" t="inlineStr"/>
@@ -3639,7 +3639,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>73756</t>
+          <t>73757</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -3657,12 +3657,12 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>地理 -- GEOG</t>
+          <t>數學 -- MATH</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>作業</t>
+          <t>HW 2C</t>
         </is>
       </c>
       <c r="G104" t="inlineStr"/>
@@ -3887,12 +3887,12 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>73886</t>
+          <t>73824</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="C112" s="2" t="n">
@@ -3905,12 +3905,12 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>數學 -- MATH</t>
+          <t>英文 -- ENG</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>CW 23</t>
+          <t>FT Revison</t>
         </is>
       </c>
       <c r="G112" t="inlineStr"/>
@@ -3918,12 +3918,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>73824</t>
+          <t>73886</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="C113" s="2" t="n">
@@ -3936,12 +3936,12 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>英文 -- ENG</t>
+          <t>數學 -- MATH</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>FT Revison</t>
+          <t>CW 23</t>
         </is>
       </c>
       <c r="G113" t="inlineStr"/>
@@ -4197,7 +4197,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>73985</t>
+          <t>73984</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -4215,12 +4215,12 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>數學 -- MATH</t>
+          <t>科學 -- SCI</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>UT Paper Corr + Sign</t>
+          <t>WB p16, 20</t>
         </is>
       </c>
       <c r="G122" t="inlineStr"/>
@@ -4259,7 +4259,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>73984</t>
+          <t>73985</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -4277,12 +4277,12 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>科學 -- SCI</t>
+          <t>數學 -- MATH</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>WB p16, 20</t>
+          <t>UT Paper Corr + Sign</t>
         </is>
       </c>
       <c r="G124" t="inlineStr"/>
@@ -4476,12 +4476,12 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>74190</t>
+          <t>74182</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>2025-11-11</t>
+          <t>2025-11-10</t>
         </is>
       </c>
       <c r="C131" s="2" t="n">
@@ -4494,12 +4494,12 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>數學 -- MATH</t>
+          <t>普話 -- PTH</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>HW 3A</t>
+          <t>第一次語文知識驗（VLE）</t>
         </is>
       </c>
       <c r="G131" t="inlineStr"/>
@@ -4507,12 +4507,12 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>74182</t>
+          <t>74190</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>2025-11-10</t>
+          <t>2025-11-11</t>
         </is>
       </c>
       <c r="C132" s="2" t="n">
@@ -4525,12 +4525,12 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>普話 -- PTH</t>
+          <t>數學 -- MATH</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>第一次語文知識驗（VLE）</t>
+          <t>HW 3A</t>
         </is>
       </c>
       <c r="G132" t="inlineStr"/>
@@ -4538,7 +4538,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>記事6700</t>
+          <t>記事6698</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -4556,12 +4556,12 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>地理 -- GEOG</t>
+          <t>中文 -- CHIN</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>書p.41</t>
+          <t>明日圖書課，自行集隊（12:55）</t>
         </is>
       </c>
       <c r="G133" t="inlineStr"/>
@@ -4569,7 +4569,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>記事6698</t>
+          <t>記事6699</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -4587,12 +4587,12 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>中文 -- CHIN</t>
+          <t>數學 -- MATH</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>明日圖書課，自行集隊（12:55）</t>
+          <t>HW3A</t>
         </is>
       </c>
       <c r="G134" t="inlineStr"/>
@@ -4600,7 +4600,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>記事6699</t>
+          <t>記事6700</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -4618,12 +4618,12 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>數學 -- MATH</t>
+          <t>地理 -- GEOG</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>HW3A</t>
+          <t>書p.41</t>
         </is>
       </c>
       <c r="G135" t="inlineStr"/>
@@ -5166,12 +5166,12 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>74330</t>
+          <t>74373</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>2025-11-14</t>
+          <t>2025-11-17</t>
         </is>
       </c>
       <c r="C153" s="2" t="n">
@@ -5184,29 +5184,25 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>英文 -- ENG</t>
+          <t>科學 -- SCI</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
         <is>
-          <t>Solid Memory</t>
-        </is>
-      </c>
-      <c r="G153" t="inlineStr">
-        <is>
-          <t>1 Exercise 1 Day</t>
-        </is>
-      </c>
+          <t>Science book report</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>74373</t>
+          <t>74329</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>2025-11-17</t>
+          <t>2025-11-14</t>
         </is>
       </c>
       <c r="C154" s="2" t="n">
@@ -5219,12 +5215,12 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>科學 -- SCI</t>
+          <t>數學 -- MATH</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>Science book report</t>
+          <t>CW32</t>
         </is>
       </c>
       <c r="G154" t="inlineStr"/>
@@ -5232,7 +5228,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>74329</t>
+          <t>74330</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -5250,15 +5246,19 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>數學 -- MATH</t>
+          <t>英文 -- ENG</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>CW32</t>
-        </is>
-      </c>
-      <c r="G155" t="inlineStr"/>
+          <t>Solid Memory</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>1 Exercise 1 Day</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -5294,7 +5294,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>74349</t>
+          <t>74347</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -5312,20 +5312,24 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>中文 -- CHIN</t>
+          <t>公經社 -- CES</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>木蘭辭話劇</t>
-        </is>
-      </c>
-      <c r="G157" t="inlineStr"/>
+          <t>評分功課</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>連file</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>74347</t>
+          <t>74348</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -5343,24 +5347,20 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>公經社 -- CES</t>
+          <t>中文 -- CHIN</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>評分功課</t>
-        </is>
-      </c>
-      <c r="G158" t="inlineStr">
-        <is>
-          <t>連file</t>
-        </is>
-      </c>
+          <t>步步升3</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>74348</t>
+          <t>74349</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -5383,7 +5383,7 @@
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t>步步升3</t>
+          <t>木蘭辭話劇</t>
         </is>
       </c>
       <c r="G159" t="inlineStr"/>
@@ -5554,7 +5554,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>74428</t>
+          <t>74430</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -5572,24 +5572,20 @@
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>英文 -- ENG</t>
+          <t>中文 -- CHIN</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>VLE Ex 5-8</t>
-        </is>
-      </c>
-      <c r="G165" t="inlineStr">
-        <is>
-          <t>Ex5-8 Today Ex7-8 Tmr</t>
-        </is>
-      </c>
+          <t>默書簽名</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>74430</t>
+          <t>74429</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -5607,12 +5603,12 @@
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>中文 -- CHIN</t>
+          <t>英文 -- ENG</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>默書簽名</t>
+          <t>GB p.131</t>
         </is>
       </c>
       <c r="G166" t="inlineStr"/>
@@ -5620,7 +5616,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>74429</t>
+          <t>74426</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -5638,12 +5634,12 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>英文 -- ENG</t>
+          <t>數學 -- MATH</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>GB p.131</t>
+          <t>HW4A + HW Book Corr</t>
         </is>
       </c>
       <c r="G167" t="inlineStr"/>
@@ -5651,7 +5647,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>74426</t>
+          <t>74428</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -5669,25 +5665,29 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>數學 -- MATH</t>
+          <t>英文 -- ENG</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>HW4A + HW Book Corr</t>
-        </is>
-      </c>
-      <c r="G168" t="inlineStr"/>
+          <t>VLE Ex 5-8</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>Ex5-8 Today Ex7-8 Tmr</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>記事6744</t>
+          <t>74496</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>2025-11-18</t>
+          <t>2025-11-20</t>
         </is>
       </c>
       <c r="C169" s="2" t="n">
@@ -5700,33 +5700,29 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>英文 -- ENG</t>
+          <t>中文 -- CHIN</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>Listening Test</t>
-        </is>
-      </c>
-      <c r="G169" t="inlineStr">
-        <is>
-          <t>21/11</t>
-        </is>
-      </c>
+          <t>作文改正</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>74345</t>
+          <t>74497</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>2025-11-14</t>
+          <t>2025-11-20</t>
         </is>
       </c>
       <c r="C170" s="2" t="n">
-        <v>45986</v>
+        <v>45982</v>
       </c>
       <c r="D170" t="inlineStr">
         <is>
@@ -5735,33 +5731,33 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>公經社 -- CES</t>
+          <t>中文 -- CHIN</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>級測</t>
+          <t>筆記</t>
         </is>
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>放學後（40mins）</t>
+          <t>兩頁</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>記事6741</t>
+          <t>74498</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>2025-11-17</t>
+          <t>2025-11-20</t>
         </is>
       </c>
       <c r="C171" s="2" t="n">
-        <v>45987</v>
+        <v>45982</v>
       </c>
       <c r="D171" t="inlineStr">
         <is>
@@ -5770,12 +5766,12 @@
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>中文 -- CHIN</t>
+          <t>地理 -- GEOG</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>背默《木蘭辭》1-2段，創默3段</t>
+          <t>作業 p.21</t>
         </is>
       </c>
       <c r="G171" t="inlineStr"/>
@@ -5783,33 +5779,165 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
+          <t>74495</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>2025-11-20</t>
+        </is>
+      </c>
+      <c r="C172" s="2" t="n">
+        <v>45982</v>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>全班</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>英文 -- ENG</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>GB p.133 135-138</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr"/>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>記事6744</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>2025-11-18</t>
+        </is>
+      </c>
+      <c r="C173" s="2" t="n">
+        <v>45982</v>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>全班</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>英文 -- ENG</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>Listening Test</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>21/11</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>74345</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>2025-11-14</t>
+        </is>
+      </c>
+      <c r="C174" s="2" t="n">
+        <v>45986</v>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>全班</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>公經社 -- CES</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>級測</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>放學後（40mins）</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>記事6741</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>2025-11-17</t>
+        </is>
+      </c>
+      <c r="C175" s="2" t="n">
+        <v>45987</v>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>全班</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>中文 -- CHIN</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>背默《木蘭辭》1-2段，創默3段</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr"/>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
           <t>74331</t>
         </is>
       </c>
-      <c r="B172" t="inlineStr">
+      <c r="B176" t="inlineStr">
         <is>
           <t>2025-11-14</t>
         </is>
       </c>
-      <c r="C172" s="2" t="n">
+      <c r="C176" s="2" t="n">
         <v>46008</v>
       </c>
-      <c r="D172" t="inlineStr">
-        <is>
-          <t>全班</t>
-        </is>
-      </c>
-      <c r="E172" t="inlineStr">
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>全班</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
         <is>
           <t>英文 -- ENG</t>
         </is>
       </c>
-      <c r="F172" t="inlineStr">
+      <c r="F176" t="inlineStr">
         <is>
           <t>Raz-Kids</t>
         </is>
       </c>
-      <c r="G172" t="inlineStr">
+      <c r="G176" t="inlineStr">
         <is>
           <t>Dead Line 17/12</t>
         </is>

</xml_diff>